<commit_message>
postgres integration + models created
</commit_message>
<xml_diff>
--- a/HelloWorld.xlsx
+++ b/HelloWorld.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="52">
   <si>
     <t>Login Credentials</t>
   </si>
@@ -93,9 +93,6 @@
     <t>projectName</t>
   </si>
   <si>
-    <t>github</t>
-  </si>
-  <si>
     <t>contributors</t>
   </si>
   <si>
@@ -108,9 +105,6 @@
     <t>Name of the project</t>
   </si>
   <si>
-    <t>Link to Github repo</t>
-  </si>
-  <si>
     <t>Array of contribs</t>
   </si>
   <si>
@@ -166,6 +160,18 @@
   </si>
   <si>
     <t>HelloWorld Database Schema</t>
+  </si>
+  <si>
+    <t>repo</t>
+  </si>
+  <si>
+    <t>Link to repo</t>
+  </si>
+  <si>
+    <t>projectDescription</t>
+  </si>
+  <si>
+    <t>Short description of project</t>
   </si>
 </sst>
 </file>
@@ -237,16 +243,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -550,51 +556,51 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
+      <c r="A1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
     </row>
     <row r="5" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -615,30 +621,30 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -687,24 +693,24 @@
       </c>
     </row>
     <row r="14" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -717,13 +723,13 @@
         <v>21</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G16" s="1"/>
     </row>
@@ -732,111 +738,116 @@
         <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C17" t="s">
         <v>17</v>
       </c>
       <c r="D17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17" t="s">
         <v>39</v>
       </c>
-      <c r="E17" t="s">
-        <v>38</v>
-      </c>
-      <c r="F17" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="19" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="F21" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G21" s="1"/>
+        <v>32</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" t="s">
         <v>29</v>
       </c>
-      <c r="B22" t="s">
+      <c r="D22" t="s">
         <v>30</v>
       </c>
-      <c r="C22" t="s">
+      <c r="E22" t="s">
         <v>31</v>
       </c>
-      <c r="D22" t="s">
-        <v>32</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>33</v>
       </c>
-      <c r="F22" t="s">
-        <v>35</v>
+      <c r="G22" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
     </row>
     <row r="25" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B25" s="4"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
+      <c r="A25" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="3"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -845,37 +856,37 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B27" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C27" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A1:G3"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C5:G5"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="C15:G15"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:G20"/>
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="C25:G25"/>
-    <mergeCell ref="A1:G3"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C5:G5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>